<commit_message>
R-chart & PCA approach OK/Figures OK/describe results is missing
</commit_message>
<xml_diff>
--- a/stats1000_Memory.xlsx
+++ b/stats1000_Memory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-2720" yWindow="-23940" windowWidth="34980" windowHeight="21840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34980" windowHeight="21900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -3741,11 +3741,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2061643416"/>
-        <c:axId val="-2044712840"/>
+        <c:axId val="-2117987832"/>
+        <c:axId val="-2117990968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061643416"/>
+        <c:axId val="-2117987832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3764,7 +3764,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044712840"/>
+        <c:crossAx val="-2117990968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3772,7 +3772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2044712840"/>
+        <c:axId val="-2117990968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3795,7 +3795,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3812,7 +3811,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061643416"/>
+        <c:crossAx val="-2117987832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4065,8 +4064,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1861096808"/>
-        <c:axId val="1860904168"/>
+        <c:axId val="-2114011800"/>
+        <c:axId val="-2114006312"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4729,11 +4728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1861096808"/>
-        <c:axId val="1860904168"/>
+        <c:axId val="-2114011800"/>
+        <c:axId val="-2114006312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1861096808"/>
+        <c:axId val="-2114011800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4778,7 +4777,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860904168"/>
+        <c:crossAx val="-2114006312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4786,7 +4785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1860904168"/>
+        <c:axId val="-2114006312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4833,7 +4832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1861096808"/>
+        <c:crossAx val="-2114011800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5092,8 +5091,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1860755944"/>
-        <c:axId val="1860761576"/>
+        <c:axId val="-2114490056"/>
+        <c:axId val="-2114495768"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5683,11 +5682,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1860755944"/>
-        <c:axId val="1860761576"/>
+        <c:axId val="-2114490056"/>
+        <c:axId val="-2114495768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1860755944"/>
+        <c:axId val="-2114490056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5741,7 +5740,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860761576"/>
+        <c:crossAx val="-2114495768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5751,7 +5750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1860761576"/>
+        <c:axId val="-2114495768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5821,7 +5820,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860755944"/>
+        <c:crossAx val="-2114490056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6059,8 +6058,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="1860866712"/>
-        <c:axId val="-2070496968"/>
+        <c:axId val="-2114556504"/>
+        <c:axId val="-2114562616"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6533,11 +6532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1860866712"/>
-        <c:axId val="-2070496968"/>
+        <c:axId val="-2114556504"/>
+        <c:axId val="-2114562616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1860866712"/>
+        <c:axId val="-2114556504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6597,7 +6596,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070496968"/>
+        <c:crossAx val="-2114562616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6607,7 +6606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070496968"/>
+        <c:axId val="-2114562616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6671,7 +6670,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860866712"/>
+        <c:crossAx val="-2114556504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6903,8 +6902,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="1860478744"/>
-        <c:axId val="1860390952"/>
+        <c:axId val="-2114622312"/>
+        <c:axId val="-2114628424"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7356,11 +7355,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1860478744"/>
-        <c:axId val="1860390952"/>
+        <c:axId val="-2114622312"/>
+        <c:axId val="-2114628424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1860478744"/>
+        <c:axId val="-2114622312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7420,7 +7419,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860390952"/>
+        <c:crossAx val="-2114628424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7430,7 +7429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1860390952"/>
+        <c:axId val="-2114628424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7500,7 +7499,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860478744"/>
+        <c:crossAx val="-2114622312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7732,8 +7731,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="1861041448"/>
-        <c:axId val="1861047400"/>
+        <c:axId val="-2114684664"/>
+        <c:axId val="-2114690712"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8177,11 +8176,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1861041448"/>
-        <c:axId val="1861047400"/>
+        <c:axId val="-2114684664"/>
+        <c:axId val="-2114690712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1861041448"/>
+        <c:axId val="-2114684664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8241,7 +8240,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1861047400"/>
+        <c:crossAx val="-2114690712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8251,7 +8250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1861047400"/>
+        <c:axId val="-2114690712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8321,7 +8320,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1861041448"/>
+        <c:crossAx val="-2114684664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8553,8 +8552,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-1992734904"/>
-        <c:axId val="1860850440"/>
+        <c:axId val="-2114750936"/>
+        <c:axId val="-2114757016"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9006,11 +9005,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1992734904"/>
-        <c:axId val="1860850440"/>
+        <c:axId val="-2114750936"/>
+        <c:axId val="-2114757016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1992734904"/>
+        <c:axId val="-2114750936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9070,7 +9069,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860850440"/>
+        <c:crossAx val="-2114757016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9080,7 +9079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1860850440"/>
+        <c:axId val="-2114757016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9150,7 +9149,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1992734904"/>
+        <c:crossAx val="-2114750936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9383,8 +9382,8 @@
         </c:dLbls>
         <c:gapWidth val="500"/>
         <c:overlap val="-45"/>
-        <c:axId val="-1993266216"/>
-        <c:axId val="1860451800"/>
+        <c:axId val="-2114814312"/>
+        <c:axId val="-2114820392"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9828,11 +9827,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1993266216"/>
-        <c:axId val="1860451800"/>
+        <c:axId val="-2114814312"/>
+        <c:axId val="-2114820392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1993266216"/>
+        <c:axId val="-2114814312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9892,7 +9891,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860451800"/>
+        <c:crossAx val="-2114820392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9902,7 +9901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1860451800"/>
+        <c:axId val="-2114820392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9972,7 +9971,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1993266216"/>
+        <c:crossAx val="-2114814312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100.0"/>
@@ -10403,11 +10402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055472680"/>
-        <c:axId val="-2056164552"/>
+        <c:axId val="-2118062632"/>
+        <c:axId val="-2118065624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2055472680"/>
+        <c:axId val="-2118062632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10416,7 +10415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2056164552"/>
+        <c:crossAx val="-2118065624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10424,7 +10423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2056164552"/>
+        <c:axId val="-2118065624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10435,7 +10434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055472680"/>
+        <c:crossAx val="-2118062632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10682,8 +10681,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055314840"/>
-        <c:axId val="-2062344408"/>
+        <c:axId val="-2114466584"/>
+        <c:axId val="-2114460440"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11225,11 +11224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2055314840"/>
-        <c:axId val="-2062344408"/>
+        <c:axId val="-2114466584"/>
+        <c:axId val="-2114460440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2055314840"/>
+        <c:axId val="-2114466584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11303,7 +11302,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062344408"/>
+        <c:crossAx val="-2114460440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11313,7 +11312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062344408"/>
+        <c:axId val="-2114460440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11397,7 +11396,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055314840"/>
+        <c:crossAx val="-2114466584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11779,8 +11778,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055825016"/>
-        <c:axId val="-2044304936"/>
+        <c:axId val="-2114394696"/>
+        <c:axId val="-2114388552"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12610,11 +12609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2055825016"/>
-        <c:axId val="-2044304936"/>
+        <c:axId val="-2114394696"/>
+        <c:axId val="-2114388552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2055825016"/>
+        <c:axId val="-2114394696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12688,7 +12687,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044304936"/>
+        <c:crossAx val="-2114388552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12698,7 +12697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2044304936"/>
+        <c:axId val="-2114388552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12782,7 +12781,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055825016"/>
+        <c:crossAx val="-2114394696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13029,8 +13028,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2044155400"/>
-        <c:axId val="-1992332856"/>
+        <c:axId val="-2114329432"/>
+        <c:axId val="-2114323288"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13455,11 +13454,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2044155400"/>
-        <c:axId val="-1992332856"/>
+        <c:axId val="-2114329432"/>
+        <c:axId val="-2114323288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2044155400"/>
+        <c:axId val="-2114329432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13533,7 +13532,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1992332856"/>
+        <c:crossAx val="-2114323288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13543,7 +13542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1992332856"/>
+        <c:axId val="-2114323288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13627,7 +13626,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044155400"/>
+        <c:crossAx val="-2114329432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13868,8 +13867,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2056130248"/>
-        <c:axId val="-1993103720"/>
+        <c:axId val="-2114265400"/>
+        <c:axId val="-2114259256"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14276,11 +14275,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2056130248"/>
-        <c:axId val="-1993103720"/>
+        <c:axId val="-2114265400"/>
+        <c:axId val="-2114259256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2056130248"/>
+        <c:axId val="-2114265400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14354,7 +14353,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1993103720"/>
+        <c:crossAx val="-2114259256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14364,7 +14363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1993103720"/>
+        <c:axId val="-2114259256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14448,7 +14447,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056130248"/>
+        <c:crossAx val="-2114265400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14686,8 +14685,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055971608"/>
-        <c:axId val="-2055563800"/>
+        <c:axId val="-2114201256"/>
+        <c:axId val="-2114195112"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14717,7 +14716,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -14959,7 +14957,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -15085,11 +15082,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2055971608"/>
-        <c:axId val="-2055563800"/>
+        <c:axId val="-2114201256"/>
+        <c:axId val="-2114195112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2055971608"/>
+        <c:axId val="-2114201256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15163,7 +15160,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055563800"/>
+        <c:crossAx val="-2114195112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15173,7 +15170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055563800"/>
+        <c:axId val="-2114195112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15257,7 +15254,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055971608"/>
+        <c:crossAx val="-2114201256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15498,8 +15495,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1860915336"/>
-        <c:axId val="-2044602984"/>
+        <c:axId val="-2114137272"/>
+        <c:axId val="-2114131128"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -15529,7 +15526,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -15777,7 +15773,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -15906,11 +15901,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1860915336"/>
-        <c:axId val="-2044602984"/>
+        <c:axId val="-2114137272"/>
+        <c:axId val="-2114131128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1860915336"/>
+        <c:axId val="-2114137272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15984,7 +15979,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044602984"/>
+        <c:crossAx val="-2114131128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15994,7 +15989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2044602984"/>
+        <c:axId val="-2114131128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16078,7 +16073,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860915336"/>
+        <c:crossAx val="-2114137272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16316,8 +16311,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1860321752"/>
-        <c:axId val="1860327800"/>
+        <c:axId val="-2114073192"/>
+        <c:axId val="-2114067048"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -16347,7 +16342,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -16589,7 +16583,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -16715,11 +16708,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1860321752"/>
-        <c:axId val="1860327800"/>
+        <c:axId val="-2114073192"/>
+        <c:axId val="-2114067048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1860321752"/>
+        <c:axId val="-2114073192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16793,7 +16786,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860327800"/>
+        <c:crossAx val="-2114067048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16803,7 +16796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1860327800"/>
+        <c:axId val="-2114067048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16887,7 +16880,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860321752"/>
+        <c:crossAx val="-2114073192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18019,7 +18012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:BJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="M138" sqref="M138"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
R-chart & PCA figures updated OK
</commit_message>
<xml_diff>
--- a/stats1000_Memory.xlsx
+++ b/stats1000_Memory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34980" windowHeight="21900" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="-20840" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="132">
   <si>
     <t>JAVA</t>
   </si>
@@ -370,7 +370,55 @@
     <t>PHP &amp; JAVA</t>
   </si>
   <si>
-    <t>txt math</t>
+    <t xml:space="preserve"> [1] 0.35164213 0.53790549 0.43581364 0.19685192 0.07065593 0.45403134</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [7] 0.35120779 0.55457259 0.38966804 0.33431504 0.59231954 0.41348130</t>
+  </si>
+  <si>
+    <t>[13] 0.42421830 0.35229688 0.45709785 0.48145925 0.36905127 0.71031084</t>
+  </si>
+  <si>
+    <t>[19] 0.44166110 0.54800983 0.48418423 0.48870734 0.45969623 0.82531574</t>
+  </si>
+  <si>
+    <t>[25] 5.90052436 0.37837423 0.45993111 0.27035347 7.96009324 0.50625054</t>
+  </si>
+  <si>
+    <t>[31] 0.51406528 0.42538981 0.31510286 0.58273204 0.27544214 0.39305145</t>
+  </si>
+  <si>
+    <t>[37] 0.40482619 0.37911546 0.50794460 4.23670009 0.46319724 0.38472260</t>
+  </si>
+  <si>
+    <t>[43] 0.03986372 0.53876342 0.42813374 1.63115991 0.20322393 0.52722400</t>
+  </si>
+  <si>
+    <t>[49] 0.41428827 0.04313522 2.20811784 1.68176915 0.37676776 0.20775420</t>
+  </si>
+  <si>
+    <t>[55] 0.40177313 0.42183005 0.25905736 0.51491300 2.41179371 0.15815953</t>
+  </si>
+  <si>
+    <t>[61] 0.55430312 0.23807798 0.45414795 0.48520650 0.35496537 0.52243121</t>
+  </si>
+  <si>
+    <t>[67] 0.42894650 0.51080391 0.74284653 0.56273346 0.42768906 0.61529940</t>
+  </si>
+  <si>
+    <t>[73] 0.45026237 0.36362484 0.36588684 0.05585000 0.46752316 0.53959090</t>
+  </si>
+  <si>
+    <t>[79] 0.40865635 0.44258530 0.56932948 5.58433481 0.74844981 0.52216841</t>
+  </si>
+  <si>
+    <t>[85] 0.36665421 0.55080731 0.12071158 0.40946044 0.33505415 0.54704476</t>
+  </si>
+  <si>
+    <t>&gt; res$critSD</t>
+  </si>
+  <si>
+    <t>[1] 2.716203</t>
   </si>
 </sst>
 </file>
@@ -469,8 +517,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1577">
+  <cellStyleXfs count="1597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2075,7 +2143,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1577">
+  <cellStyles count="1597">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2864,6 +2932,16 @@
     <cellStyle name="Lien hypertexte" xfId="1571" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="1573" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="1575" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1577" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1579" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1581" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1583" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1585" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1587" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1589" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1591" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1593" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1595" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3652,6 +3730,16 @@
     <cellStyle name="Lien hypertexte visité" xfId="1572" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="1574" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="1576" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1578" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1580" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1582" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1584" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1586" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1588" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1590" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1592" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1594" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1596" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3741,11 +3829,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2117987832"/>
-        <c:axId val="-2117990968"/>
+        <c:axId val="-2096203272"/>
+        <c:axId val="-2084327448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2117987832"/>
+        <c:axId val="-2096203272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3764,7 +3852,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117990968"/>
+        <c:crossAx val="-2084327448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3772,7 +3860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117990968"/>
+        <c:axId val="-2084327448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3795,6 +3883,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3811,7 +3900,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117987832"/>
+        <c:crossAx val="-2096203272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4064,8 +4153,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114011800"/>
-        <c:axId val="-2114006312"/>
+        <c:axId val="-2071393960"/>
+        <c:axId val="-2071388472"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4728,11 +4817,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114011800"/>
-        <c:axId val="-2114006312"/>
+        <c:axId val="-2071393960"/>
+        <c:axId val="-2071388472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114011800"/>
+        <c:axId val="-2071393960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4777,7 +4866,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114006312"/>
+        <c:crossAx val="-2071388472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4785,7 +4874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114006312"/>
+        <c:axId val="-2071388472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4832,7 +4921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114011800"/>
+        <c:crossAx val="-2071393960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5091,8 +5180,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114490056"/>
-        <c:axId val="-2114495768"/>
+        <c:axId val="-2071323064"/>
+        <c:axId val="-2071317400"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5682,11 +5771,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114490056"/>
-        <c:axId val="-2114495768"/>
+        <c:axId val="-2071323064"/>
+        <c:axId val="-2071317400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114490056"/>
+        <c:axId val="-2071323064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5740,7 +5829,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114495768"/>
+        <c:crossAx val="-2071317400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5750,7 +5839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114495768"/>
+        <c:axId val="-2071317400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5820,7 +5909,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114490056"/>
+        <c:crossAx val="-2071323064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6058,8 +6147,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2114556504"/>
-        <c:axId val="-2114562616"/>
+        <c:axId val="-2071246200"/>
+        <c:axId val="-2093548568"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6532,11 +6621,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114556504"/>
-        <c:axId val="-2114562616"/>
+        <c:axId val="-2071246200"/>
+        <c:axId val="-2093548568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114556504"/>
+        <c:axId val="-2071246200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6596,7 +6685,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114562616"/>
+        <c:crossAx val="-2093548568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6606,7 +6695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114562616"/>
+        <c:axId val="-2093548568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6670,7 +6759,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114556504"/>
+        <c:crossAx val="-2071246200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6902,8 +6991,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2114622312"/>
-        <c:axId val="-2114628424"/>
+        <c:axId val="-2093432248"/>
+        <c:axId val="-2105911336"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7355,11 +7444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114622312"/>
-        <c:axId val="-2114628424"/>
+        <c:axId val="-2093432248"/>
+        <c:axId val="-2105911336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114622312"/>
+        <c:axId val="-2093432248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7419,7 +7508,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114628424"/>
+        <c:crossAx val="-2105911336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7429,7 +7518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114628424"/>
+        <c:axId val="-2105911336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7499,7 +7588,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114622312"/>
+        <c:crossAx val="-2093432248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7731,8 +7820,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2114684664"/>
-        <c:axId val="-2114690712"/>
+        <c:axId val="-2093210104"/>
+        <c:axId val="-2093227832"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8176,11 +8265,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114684664"/>
-        <c:axId val="-2114690712"/>
+        <c:axId val="-2093210104"/>
+        <c:axId val="-2093227832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114684664"/>
+        <c:axId val="-2093210104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8240,7 +8329,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114690712"/>
+        <c:crossAx val="-2093227832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8250,7 +8339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114690712"/>
+        <c:axId val="-2093227832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8320,7 +8409,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114684664"/>
+        <c:crossAx val="-2093210104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8552,8 +8641,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2114750936"/>
-        <c:axId val="-2114757016"/>
+        <c:axId val="-2093166056"/>
+        <c:axId val="-2093222472"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9005,11 +9094,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114750936"/>
-        <c:axId val="-2114757016"/>
+        <c:axId val="-2093166056"/>
+        <c:axId val="-2093222472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114750936"/>
+        <c:axId val="-2093166056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9069,7 +9158,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114757016"/>
+        <c:crossAx val="-2093222472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9079,7 +9168,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114757016"/>
+        <c:axId val="-2093222472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9149,7 +9238,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114750936"/>
+        <c:crossAx val="-2093166056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9382,8 +9471,8 @@
         </c:dLbls>
         <c:gapWidth val="500"/>
         <c:overlap val="-45"/>
-        <c:axId val="-2114814312"/>
-        <c:axId val="-2114820392"/>
+        <c:axId val="-2093314488"/>
+        <c:axId val="-2093324568"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9827,11 +9916,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114814312"/>
-        <c:axId val="-2114820392"/>
+        <c:axId val="-2093314488"/>
+        <c:axId val="-2093324568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114814312"/>
+        <c:axId val="-2093314488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9891,7 +9980,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114820392"/>
+        <c:crossAx val="-2093324568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9901,7 +9990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114820392"/>
+        <c:axId val="-2093324568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9971,7 +10060,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114814312"/>
+        <c:crossAx val="-2093314488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100.0"/>
@@ -10402,11 +10491,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2118062632"/>
-        <c:axId val="-2118065624"/>
+        <c:axId val="-2097121096"/>
+        <c:axId val="-2097118120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2118062632"/>
+        <c:axId val="-2097121096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10415,7 +10504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118065624"/>
+        <c:crossAx val="-2097118120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10423,7 +10512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118065624"/>
+        <c:axId val="-2097118120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10434,7 +10523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118062632"/>
+        <c:crossAx val="-2097121096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10681,8 +10770,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114466584"/>
-        <c:axId val="-2114460440"/>
+        <c:axId val="-2071207192"/>
+        <c:axId val="-2071179096"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11224,11 +11313,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114466584"/>
-        <c:axId val="-2114460440"/>
+        <c:axId val="-2071207192"/>
+        <c:axId val="-2071179096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114466584"/>
+        <c:axId val="-2071207192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11302,7 +11391,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114460440"/>
+        <c:crossAx val="-2071179096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11312,7 +11401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114460440"/>
+        <c:axId val="-2071179096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11396,7 +11485,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114466584"/>
+        <c:crossAx val="-2071207192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11778,8 +11867,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114394696"/>
-        <c:axId val="-2114388552"/>
+        <c:axId val="-2085939384"/>
+        <c:axId val="-2096123032"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12609,11 +12698,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114394696"/>
-        <c:axId val="-2114388552"/>
+        <c:axId val="-2085939384"/>
+        <c:axId val="-2096123032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114394696"/>
+        <c:axId val="-2085939384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12687,7 +12776,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114388552"/>
+        <c:crossAx val="-2096123032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12697,7 +12786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114388552"/>
+        <c:axId val="-2096123032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12781,7 +12870,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114394696"/>
+        <c:crossAx val="-2085939384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13028,8 +13117,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114329432"/>
-        <c:axId val="-2114323288"/>
+        <c:axId val="-2083747400"/>
+        <c:axId val="-2085832984"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13454,11 +13543,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114329432"/>
-        <c:axId val="-2114323288"/>
+        <c:axId val="-2083747400"/>
+        <c:axId val="-2085832984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114329432"/>
+        <c:axId val="-2083747400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13532,7 +13621,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114323288"/>
+        <c:crossAx val="-2085832984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13542,7 +13631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114323288"/>
+        <c:axId val="-2085832984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13626,7 +13715,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114329432"/>
+        <c:crossAx val="-2083747400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13867,8 +13956,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114265400"/>
-        <c:axId val="-2114259256"/>
+        <c:axId val="-2093993112"/>
+        <c:axId val="-2071459880"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14275,11 +14364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114265400"/>
-        <c:axId val="-2114259256"/>
+        <c:axId val="-2093993112"/>
+        <c:axId val="-2071459880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114265400"/>
+        <c:axId val="-2093993112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14353,7 +14442,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114259256"/>
+        <c:crossAx val="-2071459880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14363,7 +14452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114259256"/>
+        <c:axId val="-2071459880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14447,7 +14536,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114265400"/>
+        <c:crossAx val="-2093993112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14685,8 +14774,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114201256"/>
-        <c:axId val="-2114195112"/>
+        <c:axId val="-2071399656"/>
+        <c:axId val="-2071472744"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14716,6 +14805,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -14957,6 +15047,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -15082,11 +15173,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114201256"/>
-        <c:axId val="-2114195112"/>
+        <c:axId val="-2071399656"/>
+        <c:axId val="-2071472744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114201256"/>
+        <c:axId val="-2071399656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15160,7 +15251,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114195112"/>
+        <c:crossAx val="-2071472744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15170,7 +15261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114195112"/>
+        <c:axId val="-2071472744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15254,7 +15345,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114201256"/>
+        <c:crossAx val="-2071399656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15495,8 +15586,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114137272"/>
-        <c:axId val="-2114131128"/>
+        <c:axId val="-2093987832"/>
+        <c:axId val="-2105957512"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -15526,6 +15617,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -15773,6 +15865,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -15901,11 +15994,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114137272"/>
-        <c:axId val="-2114131128"/>
+        <c:axId val="-2093987832"/>
+        <c:axId val="-2105957512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114137272"/>
+        <c:axId val="-2093987832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15979,7 +16072,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114131128"/>
+        <c:crossAx val="-2105957512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15989,7 +16082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114131128"/>
+        <c:axId val="-2105957512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16073,7 +16166,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114137272"/>
+        <c:crossAx val="-2093987832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16311,8 +16404,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114073192"/>
-        <c:axId val="-2114067048"/>
+        <c:axId val="-2107559816"/>
+        <c:axId val="-2084039160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -16342,6 +16435,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -16583,6 +16677,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -16708,11 +16803,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114073192"/>
-        <c:axId val="-2114067048"/>
+        <c:axId val="-2107559816"/>
+        <c:axId val="-2084039160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114073192"/>
+        <c:axId val="-2107559816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16786,7 +16881,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114067048"/>
+        <c:crossAx val="-2084039160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16796,7 +16891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114067048"/>
+        <c:axId val="-2084039160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16880,7 +16975,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114073192"/>
+        <c:crossAx val="-2107559816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17576,11 +17671,6 @@
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
-        <row r="7">
-          <cell r="G7">
-            <v>1.7034813925570229</v>
-          </cell>
-        </row>
         <row r="87">
           <cell r="J87">
             <v>0</v>
@@ -18010,10 +18100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:BJ158"/>
+  <dimension ref="A6:BJ172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="M138" sqref="M138"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="I173" sqref="I173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26058,9 +26148,7 @@
         <v>0</v>
       </c>
       <c r="L137" s="4"/>
-      <c r="M137" s="4" t="s">
-        <v>115</v>
-      </c>
+      <c r="M137" s="4"/>
       <c r="N137" s="4"/>
       <c r="O137" s="4"/>
       <c r="P137" s="4"/>
@@ -26695,16 +26783,95 @@
       <c r="AR155" s="2"/>
     </row>
     <row r="156" spans="1:62">
+      <c r="L156" t="s">
+        <v>115</v>
+      </c>
       <c r="AQ156" s="2"/>
       <c r="AR156" s="2"/>
     </row>
     <row r="157" spans="1:62">
+      <c r="L157" t="s">
+        <v>116</v>
+      </c>
       <c r="AQ157" s="2"/>
       <c r="AR157" s="2"/>
     </row>
     <row r="158" spans="1:62">
+      <c r="L158" t="s">
+        <v>117</v>
+      </c>
       <c r="AQ158" s="2"/>
       <c r="AR158" s="2"/>
+    </row>
+    <row r="159" spans="1:62">
+      <c r="L159" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="160" spans="1:62">
+      <c r="L160" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="161" spans="12:12">
+      <c r="L161" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="162" spans="12:12">
+      <c r="L162" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="163" spans="12:12">
+      <c r="L163" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="164" spans="12:12">
+      <c r="L164" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="165" spans="12:12">
+      <c r="L165" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="166" spans="12:12">
+      <c r="L166" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="167" spans="12:12">
+      <c r="L167" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="168" spans="12:12">
+      <c r="L168" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="169" spans="12:12">
+      <c r="L169" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="170" spans="12:12">
+      <c r="L170" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="171" spans="12:12">
+      <c r="L171" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="172" spans="12:12">
+      <c r="L172" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Chapter 4: R-chart results description OK
</commit_message>
<xml_diff>
--- a/stats1000_Memory.xlsx
+++ b/stats1000_Memory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="-20840" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="-5440" yWindow="-18980" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -517,8 +517,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1597">
+  <cellStyleXfs count="1603">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2143,7 +2149,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1597">
+  <cellStyles count="1603">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2942,6 +2948,9 @@
     <cellStyle name="Lien hypertexte" xfId="1591" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="1593" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="1595" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1597" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1599" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1601" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3740,6 +3749,9 @@
     <cellStyle name="Lien hypertexte visité" xfId="1592" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="1594" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="1596" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1598" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1600" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="1602" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3829,11 +3841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2096203272"/>
-        <c:axId val="-2084327448"/>
+        <c:axId val="-2107744600"/>
+        <c:axId val="-2107741768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096203272"/>
+        <c:axId val="-2107744600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3852,7 +3864,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084327448"/>
+        <c:crossAx val="-2107741768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3860,7 +3872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2084327448"/>
+        <c:axId val="-2107741768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3900,7 +3912,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096203272"/>
+        <c:crossAx val="-2107744600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4153,8 +4165,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071393960"/>
-        <c:axId val="-2071388472"/>
+        <c:axId val="-2064616712"/>
+        <c:axId val="-2064014888"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4817,11 +4829,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2071393960"/>
-        <c:axId val="-2071388472"/>
+        <c:axId val="-2064616712"/>
+        <c:axId val="-2064014888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2071393960"/>
+        <c:axId val="-2064616712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4866,7 +4878,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071388472"/>
+        <c:crossAx val="-2064014888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4874,7 +4886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071388472"/>
+        <c:axId val="-2064014888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,7 +4914,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Performance variation</a:t>
+                  <a:t>Memory usage variation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4921,7 +4933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071393960"/>
+        <c:crossAx val="-2064616712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5180,8 +5192,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071323064"/>
-        <c:axId val="-2071317400"/>
+        <c:axId val="-2063617640"/>
+        <c:axId val="-2064357512"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5771,11 +5783,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2071323064"/>
-        <c:axId val="-2071317400"/>
+        <c:axId val="-2063617640"/>
+        <c:axId val="-2064357512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2071323064"/>
+        <c:axId val="-2063617640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5829,7 +5841,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071317400"/>
+        <c:crossAx val="-2064357512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5839,7 +5851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071317400"/>
+        <c:axId val="-2064357512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5866,7 +5878,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Performance variation</a:t>
+                  <a:t>Memory usage variation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5909,7 +5921,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071323064"/>
+        <c:crossAx val="-2063617640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6147,8 +6159,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2071246200"/>
-        <c:axId val="-2093548568"/>
+        <c:axId val="-2063979496"/>
+        <c:axId val="2040750824"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6621,11 +6633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2071246200"/>
-        <c:axId val="-2093548568"/>
+        <c:axId val="-2063979496"/>
+        <c:axId val="2040750824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2071246200"/>
+        <c:axId val="-2063979496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6685,7 +6697,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093548568"/>
+        <c:crossAx val="2040750824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6695,7 +6707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093548568"/>
+        <c:axId val="2040750824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6721,9 +6733,12 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>Performance variation</a:t>
+                  <a:rPr lang="fr-FR" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Memory usage variation</a:t>
                 </a:r>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6759,7 +6774,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071246200"/>
+        <c:crossAx val="-2063979496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6991,8 +7006,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2093432248"/>
-        <c:axId val="-2105911336"/>
+        <c:axId val="-2088888680"/>
+        <c:axId val="-2088876952"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7444,11 +7459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093432248"/>
-        <c:axId val="-2105911336"/>
+        <c:axId val="-2088888680"/>
+        <c:axId val="-2088876952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093432248"/>
+        <c:axId val="-2088888680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7508,7 +7523,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105911336"/>
+        <c:crossAx val="-2088876952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7518,7 +7533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105911336"/>
+        <c:axId val="-2088876952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7544,8 +7559,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="fr-FR" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Memory usage </a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Performance variation</a:t>
+                  <a:t>variation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7588,7 +7609,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093432248"/>
+        <c:crossAx val="-2088888680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7820,8 +7841,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2093210104"/>
-        <c:axId val="-2093227832"/>
+        <c:axId val="-2089376760"/>
+        <c:axId val="-2089390280"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8265,11 +8286,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093210104"/>
-        <c:axId val="-2093227832"/>
+        <c:axId val="-2089376760"/>
+        <c:axId val="-2089390280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093210104"/>
+        <c:axId val="-2089376760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8329,7 +8350,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093227832"/>
+        <c:crossAx val="-2089390280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8339,7 +8360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093227832"/>
+        <c:axId val="-2089390280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8365,8 +8386,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="fr-FR" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Memory usage </a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Performance variation</a:t>
+                  <a:t>variation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8409,7 +8436,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093210104"/>
+        <c:crossAx val="-2089376760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8641,8 +8668,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-2093166056"/>
-        <c:axId val="-2093222472"/>
+        <c:axId val="-2061419576"/>
+        <c:axId val="-2060709272"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9094,11 +9121,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093166056"/>
-        <c:axId val="-2093222472"/>
+        <c:axId val="-2061419576"/>
+        <c:axId val="-2060709272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093166056"/>
+        <c:axId val="-2061419576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9158,7 +9185,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093222472"/>
+        <c:crossAx val="-2060709272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9168,7 +9195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093222472"/>
+        <c:axId val="-2060709272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9194,8 +9221,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="fr-FR" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Memory usage </a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Perforamnce variation</a:t>
+                  <a:t>variation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9238,7 +9271,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093166056"/>
+        <c:crossAx val="-2061419576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9471,8 +9504,8 @@
         </c:dLbls>
         <c:gapWidth val="500"/>
         <c:overlap val="-45"/>
-        <c:axId val="-2093314488"/>
-        <c:axId val="-2093324568"/>
+        <c:axId val="-2060979448"/>
+        <c:axId val="-2061231320"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9916,11 +9949,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093314488"/>
-        <c:axId val="-2093324568"/>
+        <c:axId val="-2060979448"/>
+        <c:axId val="-2061231320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093314488"/>
+        <c:axId val="-2060979448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9980,7 +10013,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093324568"/>
+        <c:crossAx val="-2061231320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9990,7 +10023,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093324568"/>
+        <c:axId val="-2061231320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10016,8 +10049,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="fr-FR" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Memory usage </a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Performance variation</a:t>
+                  <a:t>variation</a:t>
                 </a:r>
               </a:p>
               <a:p>
@@ -10060,7 +10099,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093314488"/>
+        <c:crossAx val="-2060979448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100.0"/>
@@ -10491,11 +10530,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2097121096"/>
-        <c:axId val="-2097118120"/>
+        <c:axId val="-2108576536"/>
+        <c:axId val="-2108573688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2097121096"/>
+        <c:axId val="-2108576536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10504,7 +10543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2097118120"/>
+        <c:crossAx val="-2108573688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10512,7 +10551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097118120"/>
+        <c:axId val="-2108573688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10523,7 +10562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2097121096"/>
+        <c:crossAx val="-2108576536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10770,8 +10809,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071207192"/>
-        <c:axId val="-2071179096"/>
+        <c:axId val="-2108346440"/>
+        <c:axId val="-2108238744"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11313,11 +11352,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2071207192"/>
-        <c:axId val="-2071179096"/>
+        <c:axId val="-2108346440"/>
+        <c:axId val="-2108238744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2071207192"/>
+        <c:axId val="-2108346440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11391,7 +11430,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071179096"/>
+        <c:crossAx val="-2108238744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11401,7 +11440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071179096"/>
+        <c:axId val="-2108238744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11485,7 +11524,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071207192"/>
+        <c:crossAx val="-2108346440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11867,8 +11906,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2085939384"/>
-        <c:axId val="-2096123032"/>
+        <c:axId val="-2089033352"/>
+        <c:axId val="-2089298728"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12698,11 +12737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2085939384"/>
-        <c:axId val="-2096123032"/>
+        <c:axId val="-2089033352"/>
+        <c:axId val="-2089298728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2085939384"/>
+        <c:axId val="-2089033352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12776,7 +12815,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096123032"/>
+        <c:crossAx val="-2089298728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12786,7 +12825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096123032"/>
+        <c:axId val="-2089298728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12870,7 +12909,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085939384"/>
+        <c:crossAx val="-2089033352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13117,8 +13156,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2083747400"/>
-        <c:axId val="-2085832984"/>
+        <c:axId val="-2119027768"/>
+        <c:axId val="-2089163992"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13543,11 +13582,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2083747400"/>
-        <c:axId val="-2085832984"/>
+        <c:axId val="-2119027768"/>
+        <c:axId val="-2089163992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2083747400"/>
+        <c:axId val="-2119027768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13621,7 +13660,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085832984"/>
+        <c:crossAx val="-2089163992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13631,7 +13670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2085832984"/>
+        <c:axId val="-2089163992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13715,7 +13754,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083747400"/>
+        <c:crossAx val="-2119027768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13956,8 +13995,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2093993112"/>
-        <c:axId val="-2071459880"/>
+        <c:axId val="-2119113832"/>
+        <c:axId val="-2089010296"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14364,11 +14403,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093993112"/>
-        <c:axId val="-2071459880"/>
+        <c:axId val="-2119113832"/>
+        <c:axId val="-2089010296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093993112"/>
+        <c:axId val="-2119113832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14442,7 +14481,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071459880"/>
+        <c:crossAx val="-2089010296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14452,7 +14491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071459880"/>
+        <c:axId val="-2089010296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14536,7 +14575,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093993112"/>
+        <c:crossAx val="-2119113832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14774,8 +14813,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071399656"/>
-        <c:axId val="-2071472744"/>
+        <c:axId val="-2089106840"/>
+        <c:axId val="-2088972024"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -15173,11 +15212,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2071399656"/>
-        <c:axId val="-2071472744"/>
+        <c:axId val="-2089106840"/>
+        <c:axId val="-2088972024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2071399656"/>
+        <c:axId val="-2089106840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15251,7 +15290,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071472744"/>
+        <c:crossAx val="-2088972024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15261,7 +15300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071472744"/>
+        <c:axId val="-2088972024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15345,7 +15384,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071399656"/>
+        <c:crossAx val="-2089106840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15586,8 +15625,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2093987832"/>
-        <c:axId val="-2105957512"/>
+        <c:axId val="-2118330776"/>
+        <c:axId val="-2118984232"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -15994,11 +16033,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093987832"/>
-        <c:axId val="-2105957512"/>
+        <c:axId val="-2118330776"/>
+        <c:axId val="-2118984232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093987832"/>
+        <c:axId val="-2118330776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16072,7 +16111,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105957512"/>
+        <c:crossAx val="-2118984232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16082,7 +16121,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105957512"/>
+        <c:axId val="-2118984232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16166,7 +16205,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093987832"/>
+        <c:crossAx val="-2118330776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16404,8 +16443,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2107559816"/>
-        <c:axId val="-2084039160"/>
+        <c:axId val="-2063924808"/>
+        <c:axId val="-2064365448"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -16803,11 +16842,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2107559816"/>
-        <c:axId val="-2084039160"/>
+        <c:axId val="-2063924808"/>
+        <c:axId val="-2064365448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2107559816"/>
+        <c:axId val="-2063924808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16881,7 +16920,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084039160"/>
+        <c:crossAx val="-2064365448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16891,7 +16930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2084039160"/>
+        <c:axId val="-2064365448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16975,7 +17014,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107559816"/>
+        <c:crossAx val="-2063924808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17669,7 +17708,7 @@
       <sheetName val="Feuil2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="87">
           <cell r="J87">
@@ -17772,7 +17811,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -18102,8 +18141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:BJ172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I173" sqref="I173"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="R143" sqref="R143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>